<commit_message>
more cleanup on all_features
</commit_message>
<xml_diff>
--- a/all_features/all_features.xlsx
+++ b/all_features/all_features.xlsx
@@ -514,7 +514,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C65"/>
   <sheetData>
     <row r="1" spans="1:3" customFormat="false">
       <c r="A1" s="0" t="str">
@@ -559,339 +559,415 @@
       <c r="C6" s="0"/>
     </row>
     <row r="7" spans="1:3" customFormat="false">
-      <c r="A7" s="0" t="str">
-        <v>borderstyle</v>
-      </c>
+      <c r="A7" s="0"/>
       <c r="B7" s="0"/>
       <c r="C7" s="0"/>
     </row>
     <row r="8" spans="1:3" customFormat="false">
-      <c r="A8" s="0"/>
-      <c r="B8" s="11" t="str">
-        <v>border=all/borderstyle=dashed</v>
-      </c>
+      <c r="A8" s="0" t="str">
+        <v>borderstyle</v>
+      </c>
+      <c r="B8" s="0"/>
       <c r="C8" s="0"/>
     </row>
     <row r="9" spans="1:3" customFormat="false">
       <c r="A9" s="0"/>
-      <c r="B9" s="7" t="str">
+      <c r="B9" s="11" t="str">
+        <v>border=all/borderstyle=dashed</v>
+      </c>
+      <c r="C9" s="0"/>
+    </row>
+    <row r="10" spans="1:3" customFormat="false">
+      <c r="A10" s="0"/>
+      <c r="B10" s="7" t="str">
         <v>border=all/borderstyle=solid</v>
       </c>
-      <c r="C9" s="0"/>
-    </row>
-    <row r="10" spans="1:3" customFormat="false">
-      <c r="A10" s="0" t="str">
-        <v>color</v>
-      </c>
-      <c r="B10" s="0"/>
       <c r="C10" s="0"/>
     </row>
     <row r="11" spans="1:3" customFormat="false">
       <c r="A11" s="0"/>
-      <c r="B11" s="12" t="str">
+      <c r="B11" s="0"/>
+      <c r="C11" s="0"/>
+    </row>
+    <row r="12" spans="1:3" customFormat="false">
+      <c r="A12" s="0" t="str">
+        <v>color</v>
+      </c>
+      <c r="B12" s="0"/>
+      <c r="C12" s="0"/>
+    </row>
+    <row r="13" spans="1:3" customFormat="false">
+      <c r="A13" s="0"/>
+      <c r="B13" s="12" t="str">
         <v>color=FF0000</v>
       </c>
-      <c r="C11" s="0"/>
-    </row>
-    <row r="12" spans="1:3" customFormat="false">
-      <c r="A12" s="0"/>
-      <c r="B12" s="13" t="str">
-        <v>color=ABC</v>
-      </c>
-      <c r="C12" s="0"/>
-    </row>
-    <row r="13" spans="1:3" customFormat="false">
-      <c r="A13" s="0" t="str">
-        <v>expand</v>
-      </c>
-      <c r="B13" s="0"/>
       <c r="C13" s="0"/>
     </row>
     <row r="14" spans="1:3" customFormat="false">
       <c r="A14" s="0"/>
-      <c r="B14" s="0" t="str">
-        <v>expand=3</v>
+      <c r="B14" s="13" t="str">
+        <v>color=ABC</v>
       </c>
       <c r="C14" s="0"/>
     </row>
     <row r="15" spans="1:3" customFormat="false">
       <c r="A15" s="0"/>
-      <c r="B15" s="0" t="str">
+      <c r="B15" s="0"/>
+      <c r="C15" s="0"/>
+    </row>
+    <row r="16" spans="1:3" customFormat="false">
+      <c r="A16" s="0" t="str">
+        <v>expand</v>
+      </c>
+      <c r="B16" s="0"/>
+      <c r="C16" s="0"/>
+    </row>
+    <row r="17" spans="1:3" customFormat="false">
+      <c r="A17" s="0"/>
+      <c r="B17" s="0" t="str">
         <v>expand=3</v>
       </c>
-      <c r="C15" s="0"/>
-    </row>
-    <row r="16" spans="1:3" customFormat="false">
-      <c r="A16" s="0"/>
-      <c r="B16" s="0" t="str">
-        <v>expand=3</v>
-      </c>
-      <c r="C16" s="0"/>
-    </row>
-    <row r="17" spans="1:3" customFormat="false">
-      <c r="A17" s="0" t="str">
-        <v>fontcolor</v>
-      </c>
-      <c r="B17" s="0"/>
       <c r="C17" s="0"/>
     </row>
     <row r="18" spans="1:3" customFormat="false">
       <c r="A18" s="0"/>
-      <c r="B18" s="14" t="str">
-        <v>fontcolor=FF0000</v>
+      <c r="B18" s="0" t="str">
+        <v>expand=3</v>
       </c>
       <c r="C18" s="0"/>
     </row>
     <row r="19" spans="1:3" customFormat="false">
       <c r="A19" s="0"/>
-      <c r="B19" s="15" t="str">
-        <v>fontcolor=ABC</v>
+      <c r="B19" s="0" t="str">
+        <v>expand=3</v>
       </c>
       <c r="C19" s="0"/>
     </row>
     <row r="20" spans="1:3" customFormat="false">
-      <c r="A20" s="0" t="str">
-        <v>fontfamily</v>
-      </c>
+      <c r="A20" s="0"/>
       <c r="B20" s="0"/>
       <c r="C20" s="0"/>
     </row>
     <row r="21" spans="1:3" customFormat="false">
-      <c r="A21" s="0"/>
-      <c r="B21" s="16" t="str">
-        <v>fontfamily='Comic Sans MS'</v>
-      </c>
+      <c r="A21" s="0" t="str">
+        <v>fontcolor</v>
+      </c>
+      <c r="B21" s="0"/>
       <c r="C21" s="0"/>
     </row>
     <row r="22" spans="1:3" customFormat="false">
       <c r="A22" s="0"/>
-      <c r="B22" s="17" t="str">
-        <v>fontfamily='Helvetica'</v>
+      <c r="B22" s="14" t="str">
+        <v>fontcolor=FF0000</v>
       </c>
       <c r="C22" s="0"/>
     </row>
     <row r="23" spans="1:3" customFormat="false">
-      <c r="A23" s="0" t="str">
-        <v>fontsize</v>
-      </c>
-      <c r="B23" s="0"/>
+      <c r="A23" s="0"/>
+      <c r="B23" s="15" t="str">
+        <v>fontcolor=ABC</v>
+      </c>
       <c r="C23" s="0"/>
     </row>
     <row r="24" spans="1:3" customFormat="false">
       <c r="A24" s="0"/>
-      <c r="B24" s="18" t="str">
-        <v>fontsize=20</v>
-      </c>
+      <c r="B24" s="0"/>
       <c r="C24" s="0"/>
     </row>
     <row r="25" spans="1:3" customFormat="false">
-      <c r="A25" s="0"/>
-      <c r="B25" s="19" t="str">
-        <v>fontsize=4</v>
-      </c>
+      <c r="A25" s="0" t="str">
+        <v>fontfamily</v>
+      </c>
+      <c r="B25" s="0"/>
       <c r="C25" s="0"/>
     </row>
     <row r="26" spans="1:3" customFormat="false">
-      <c r="A26" s="0" t="str">
-        <v>format</v>
-      </c>
-      <c r="B26" s="0"/>
+      <c r="A26" s="0"/>
+      <c r="B26" s="16" t="str">
+        <v>fontfamily='Comic Sans MS'</v>
+      </c>
       <c r="C26" s="0"/>
     </row>
     <row r="27" spans="1:3" customFormat="false">
       <c r="A27" s="0"/>
-      <c r="B27" s="20" t="str">
-        <v>format=bold</v>
+      <c r="B27" s="17" t="str">
+        <v>fontfamily='Helvetica'</v>
       </c>
       <c r="C27" s="0"/>
     </row>
     <row r="28" spans="1:3" customFormat="false">
       <c r="A28" s="0"/>
-      <c r="B28" s="21" t="str">
-        <v>format=italic</v>
-      </c>
+      <c r="B28" s="0"/>
       <c r="C28" s="0"/>
     </row>
     <row r="29" spans="1:3" customFormat="false">
-      <c r="A29" s="0"/>
-      <c r="B29" s="22" t="str">
-        <v>format=underline</v>
-      </c>
+      <c r="A29" s="0" t="str">
+        <v>fontsize</v>
+      </c>
+      <c r="B29" s="0"/>
       <c r="C29" s="0"/>
     </row>
     <row r="30" spans="1:3" customFormat="false">
       <c r="A30" s="0"/>
-      <c r="B30" s="23" t="str">
-        <v>format=strikethrough</v>
+      <c r="B30" s="18" t="str">
+        <v>fontsize=20</v>
       </c>
       <c r="C30" s="0"/>
     </row>
     <row r="31" spans="1:3" customFormat="false">
-      <c r="A31" s="0" t="str">
-        <v>halign</v>
-      </c>
-      <c r="B31" s="0"/>
+      <c r="A31" s="0"/>
+      <c r="B31" s="19" t="str">
+        <v>fontsize=4</v>
+      </c>
       <c r="C31" s="0"/>
     </row>
     <row r="32" spans="1:3" customFormat="false">
       <c r="A32" s="0"/>
-      <c r="B32" s="24" t="str">
-        <v>halign=left</v>
-      </c>
+      <c r="B32" s="0"/>
       <c r="C32" s="0"/>
     </row>
     <row r="33" spans="1:3" customFormat="false">
-      <c r="A33" s="0"/>
-      <c r="B33" s="25" t="str">
-        <v>halign=center</v>
-      </c>
+      <c r="A33" s="0" t="str">
+        <v>format</v>
+      </c>
+      <c r="B33" s="0"/>
       <c r="C33" s="0"/>
     </row>
     <row r="34" spans="1:3" customFormat="false">
       <c r="A34" s="0"/>
-      <c r="B34" s="26" t="str">
-        <v>halign=right</v>
+      <c r="B34" s="20" t="str">
+        <v>format=bold</v>
       </c>
       <c r="C34" s="0"/>
     </row>
     <row r="35" spans="1:3" customFormat="false">
-      <c r="A35" s="0" t="str">
-        <v>note</v>
-      </c>
-      <c r="B35" s="0"/>
+      <c r="A35" s="0"/>
+      <c r="B35" s="21" t="str">
+        <v>format=italic</v>
+      </c>
       <c r="C35" s="0"/>
     </row>
     <row r="36" spans="1:3" customFormat="false">
       <c r="A36" s="0"/>
-      <c r="B36" s="0" t="str">
-        <v>note='this is a note'</v>
+      <c r="B36" s="22" t="str">
+        <v>format=underline</v>
       </c>
       <c r="C36" s="0"/>
     </row>
     <row r="37" spans="1:3" customFormat="false">
-      <c r="A37" s="0" t="str">
-        <v>numberformat</v>
-      </c>
-      <c r="B37" s="0"/>
+      <c r="A37" s="0"/>
+      <c r="B37" s="23" t="str">
+        <v>format=strikethrough</v>
+      </c>
       <c r="C37" s="0"/>
     </row>
     <row r="38" spans="1:3" customFormat="false">
       <c r="A38" s="0"/>
-      <c r="B38" s="27" t="str">
-        <v>123456</v>
-      </c>
+      <c r="B38" s="0"/>
       <c r="C38" s="0"/>
     </row>
     <row r="39" spans="1:3" customFormat="false">
-      <c r="A39" s="0"/>
-      <c r="B39" s="28" t="str">
-        <v>123456</v>
-      </c>
+      <c r="A39" s="0" t="str">
+        <v>halign</v>
+      </c>
+      <c r="B39" s="0"/>
       <c r="C39" s="0"/>
     </row>
     <row r="40" spans="1:3" customFormat="false">
       <c r="A40" s="0"/>
-      <c r="B40" s="29" t="str">
-        <v>123456</v>
+      <c r="B40" s="24" t="str">
+        <v>halign=left</v>
       </c>
       <c r="C40" s="0"/>
     </row>
     <row r="41" spans="1:3" customFormat="false">
       <c r="A41" s="0"/>
-      <c r="B41" s="30" t="str">
-        <v>123456</v>
+      <c r="B41" s="25" t="str">
+        <v>halign=center</v>
       </c>
       <c r="C41" s="0"/>
     </row>
     <row r="42" spans="1:3" customFormat="false">
       <c r="A42" s="0"/>
-      <c r="B42" s="31" t="str">
-        <v>123456</v>
+      <c r="B42" s="26" t="str">
+        <v>halign=right</v>
       </c>
       <c r="C42" s="0"/>
     </row>
     <row r="43" spans="1:3" customFormat="false">
       <c r="A43" s="0"/>
-      <c r="B43" s="32" t="str">
-        <v>123456</v>
-      </c>
+      <c r="B43" s="0"/>
       <c r="C43" s="0"/>
     </row>
     <row r="44" spans="1:3" customFormat="false">
-      <c r="A44" s="0"/>
-      <c r="B44" s="33" t="str">
-        <v>123456</v>
-      </c>
+      <c r="A44" s="0" t="str">
+        <v>note</v>
+      </c>
+      <c r="B44" s="0"/>
       <c r="C44" s="0"/>
     </row>
     <row r="45" spans="1:3" customFormat="false">
       <c r="A45" s="0"/>
-      <c r="B45" s="34" t="str">
-        <v>123456</v>
+      <c r="B45" s="0" t="str">
+        <v>note='this is a note'</v>
       </c>
       <c r="C45" s="0"/>
     </row>
     <row r="46" spans="1:3" customFormat="false">
-      <c r="A46" s="0" t="str">
-        <v>valign</v>
-      </c>
+      <c r="A46" s="0"/>
       <c r="B46" s="0"/>
       <c r="C46" s="0"/>
     </row>
     <row r="47" spans="1:3" customFormat="false">
-      <c r="A47" s="0"/>
-      <c r="B47" s="35" t="str">
-        <v>valign=top</v>
-      </c>
+      <c r="A47" s="0" t="str">
+        <v>numberformat</v>
+      </c>
+      <c r="B47" s="0"/>
       <c r="C47" s="0"/>
     </row>
     <row r="48" spans="1:3" customFormat="false">
       <c r="A48" s="0"/>
-      <c r="B48" s="36" t="str">
-        <v>valign=center</v>
-      </c>
-      <c r="C48" s="0"/>
+      <c r="B48" s="0" t="str">
+        <v>numberformat=currency</v>
+      </c>
+      <c r="C48" s="27" t="str">
+        <v>123456</v>
+      </c>
     </row>
     <row r="49" spans="1:3" customFormat="false">
       <c r="A49" s="0"/>
-      <c r="B49" s="37" t="str">
-        <v>valign=bottom</v>
-      </c>
-      <c r="C49" s="0"/>
+      <c r="B49" s="0" t="str">
+        <v>numberformat=date</v>
+      </c>
+      <c r="C49" s="28" t="str">
+        <v>123456</v>
+      </c>
     </row>
     <row r="50" spans="1:3" customFormat="false">
-      <c r="A50" s="0" t="str">
-        <v>variables</v>
-      </c>
-      <c r="B50" s="0"/>
-      <c r="C50" s="0"/>
+      <c r="A50" s="0"/>
+      <c r="B50" s="0" t="str">
+        <v>numberformat=date_time</v>
+      </c>
+      <c r="C50" s="29" t="str">
+        <v>123456</v>
+      </c>
     </row>
     <row r="51" spans="1:3" customFormat="false">
       <c r="A51" s="0"/>
       <c r="B51" s="0" t="str">
-        <v>depends_on_another</v>
-      </c>
-      <c r="C51" s="0">
-        <f>(1 + 2)</f>
-        <v/>
+        <v>numberformat=number</v>
+      </c>
+      <c r="C51" s="30" t="str">
+        <v>123456</v>
       </c>
     </row>
     <row r="52" spans="1:3" customFormat="false">
       <c r="A52" s="0"/>
       <c r="B52" s="0" t="str">
-        <v>my_function()</v>
-      </c>
-      <c r="C52" s="0">
-        <f>((1 + 2) * 8)</f>
-        <v/>
+        <v>numberformat=percent</v>
+      </c>
+      <c r="C52" s="31" t="str">
+        <v>123456</v>
       </c>
     </row>
     <row r="53" spans="1:3" customFormat="false">
       <c r="A53" s="0"/>
       <c r="B53" s="0" t="str">
+        <v>numberformat=text</v>
+      </c>
+      <c r="C53" s="32" t="str">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" customFormat="false">
+      <c r="A54" s="0"/>
+      <c r="B54" s="0" t="str">
+        <v>numberformat=time</v>
+      </c>
+      <c r="C54" s="33" t="str">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" customFormat="false">
+      <c r="A55" s="0"/>
+      <c r="B55" s="0" t="str">
+        <v>numberformat=scientific</v>
+      </c>
+      <c r="C55" s="34" t="str">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" customFormat="false">
+      <c r="A56" s="0"/>
+      <c r="B56" s="0"/>
+      <c r="C56" s="0"/>
+    </row>
+    <row r="57" spans="1:3" customFormat="false">
+      <c r="A57" s="0" t="str">
+        <v>valign</v>
+      </c>
+      <c r="B57" s="0"/>
+      <c r="C57" s="0"/>
+    </row>
+    <row r="58" spans="1:3" customFormat="false">
+      <c r="A58" s="0"/>
+      <c r="B58" s="35" t="str">
+        <v>valign=top</v>
+      </c>
+      <c r="C58" s="0"/>
+    </row>
+    <row r="59" spans="1:3" customFormat="false">
+      <c r="A59" s="0"/>
+      <c r="B59" s="36" t="str">
+        <v>valign=center</v>
+      </c>
+      <c r="C59" s="0"/>
+    </row>
+    <row r="60" spans="1:3" customFormat="false">
+      <c r="A60" s="0"/>
+      <c r="B60" s="37" t="str">
+        <v>valign=bottom</v>
+      </c>
+      <c r="C60" s="0"/>
+    </row>
+    <row r="61" spans="1:3" customFormat="false">
+      <c r="A61" s="0"/>
+      <c r="B61" s="0"/>
+      <c r="C61" s="0"/>
+    </row>
+    <row r="62" spans="1:3" customFormat="false">
+      <c r="A62" s="0" t="str">
+        <v>variables</v>
+      </c>
+      <c r="B62" s="0"/>
+      <c r="C62" s="0"/>
+    </row>
+    <row r="63" spans="1:3" customFormat="false">
+      <c r="A63" s="0"/>
+      <c r="B63" s="0" t="str">
+        <v>depends_on_another</v>
+      </c>
+      <c r="C63" s="0">
+        <f>(1 + 2)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="1:3" customFormat="false">
+      <c r="A64" s="0"/>
+      <c r="B64" s="0" t="str">
+        <v>my_function()</v>
+      </c>
+      <c r="C64" s="0">
+        <f>((1 + 2) * 8)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:3" customFormat="false">
+      <c r="A65" s="0"/>
+      <c r="B65" s="0" t="str">
         <v>simple_var</v>
       </c>
-      <c r="C53" s="0">
+      <c r="C65" s="0">
         <f>1</f>
         <v/>
       </c>

</xml_diff>

<commit_message>
update to csvpp 0.3.0
</commit_message>
<xml_diff>
--- a/all_features/all_features.xlsx
+++ b/all_features/all_features.xlsx
@@ -14,6 +14,23 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A42" authorId="0">
+      <text>
+        <r>
+          <t>this is a note</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="133">
   <si>
@@ -554,9 +571,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
+    <numFmt numFmtId="176" formatCode="$#,##0_-"/>
+    <numFmt numFmtId="177" formatCode="yyyy-mm-dd"/>
     <numFmt numFmtId="178" formatCode="d/m/yy h:mm"/>
-    <numFmt numFmtId="177" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="176" formatCode="$#,##0_-"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -1534,5 +1551,6 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
each workbook gets it's own Makefile
</commit_message>
<xml_diff>
--- a/all_features/all_features.xlsx
+++ b/all_features/all_features.xlsx
@@ -253,7 +253,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="3">
+    <numFmt numFmtId="176" formatCode="$#,##0_-"/>
+    <numFmt numFmtId="178" formatCode="d/m/yy h:mm"/>
+    <numFmt numFmtId="177" formatCode="yyyy-mm-dd"/>
+  </numFmts>
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,16 +266,58 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <color rgb="AABBCCFF"/>
+    </font>
+    <font>
+      <name val="Comic Sans Ms"/>
+      <scheme val="none"/>
+    </font>
+    <font>
+      <name val="Helvetica"/>
+      <scheme val="none"/>
+    </font>
+    <font>
+      <sz val="20"/>
+    </font>
+    <font>
+      <sz val="4"/>
+    </font>
+    <font>
+      <b/>
+    </font>
+    <font>
+      <i/>
+    </font>
+    <font>
+      <u/>
+    </font>
+    <font>
+      <strike/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0000FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="AABBCCFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -278,10 +325,96 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed"/>
+      <right style="dashed"/>
+      <top style="dashed"/>
+      <bottom style="dashed"/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellXfs count="2">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="1" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellXfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -559,27 +692,27 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="5">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="6">
         <v>5</v>
       </c>
     </row>
@@ -590,12 +723,12 @@
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="7">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="6">
         <v>8</v>
       </c>
     </row>
@@ -606,12 +739,12 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="B13" t="s">
+      <c r="B13" t="s" s="8">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="B14" t="s">
+      <c r="B14" t="s" s="9">
         <v>11</v>
       </c>
     </row>
@@ -643,12 +776,12 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="B22" t="s">
+      <c r="B22" t="s" s="10">
         <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="B23" t="s">
+      <c r="B23" t="s" s="11">
         <v>16</v>
       </c>
     </row>
@@ -659,12 +792,12 @@
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="B26" t="s">
+      <c r="B26" t="s" s="12">
         <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="B27" t="s">
+      <c r="B27" t="s" s="13">
         <v>19</v>
       </c>
     </row>
@@ -675,12 +808,12 @@
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="B30" t="s">
+      <c r="B30" t="s" s="14">
         <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="B31" t="s">
+      <c r="B31" t="s" s="15">
         <v>22</v>
       </c>
     </row>
@@ -691,17 +824,17 @@
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="B34" t="s">
+      <c r="B34" t="s" s="16">
         <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="B35" t="s">
+      <c r="B35" t="s" s="17">
         <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="B36" t="s">
+      <c r="B36" t="s" s="18">
         <v>26</v>
       </c>
     </row>
@@ -726,7 +859,7 @@
       <c r="B42" t="s">
         <v>30</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="19">
         <v>123456</v>
       </c>
     </row>
@@ -734,7 +867,7 @@
       <c r="B43" t="s">
         <v>31</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" t="s" s="20">
         <v>32</v>
       </c>
     </row>
@@ -742,7 +875,7 @@
       <c r="B44" t="s">
         <v>33</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" t="s" s="21">
         <v>34</v>
       </c>
     </row>
@@ -750,7 +883,7 @@
       <c r="B45" t="s">
         <v>35</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="22">
         <v>123456</v>
       </c>
     </row>
@@ -758,7 +891,7 @@
       <c r="B46" t="s">
         <v>36</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="23">
         <v>1.23456</v>
       </c>
     </row>
@@ -766,7 +899,7 @@
       <c r="B47" t="s">
         <v>37</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="24">
         <v>123456</v>
       </c>
     </row>
@@ -774,7 +907,7 @@
       <c r="B48" t="s">
         <v>38</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" t="s" s="25">
         <v>39</v>
       </c>
     </row>
@@ -782,7 +915,7 @@
       <c r="B49" t="s">
         <v>40</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="26">
         <v>123456</v>
       </c>
     </row>
@@ -793,22 +926,22 @@
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="B52" t="s">
+      <c r="B52" t="s" s="27">
         <v>42</v>
       </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="B53" t="s">
+      <c r="B53" t="s" s="28">
         <v>43</v>
       </c>
     </row>
     <row r="54" spans="1:3">
-      <c r="B54" t="s">
+      <c r="B54" t="s" s="29">
         <v>44</v>
       </c>
     </row>
     <row r="55" spans="1:3">
-      <c r="B55" t="s">
+      <c r="B55" t="s" s="30">
         <v>45</v>
       </c>
     </row>
@@ -819,17 +952,17 @@
       </c>
     </row>
     <row r="58" spans="1:3">
-      <c r="B58" t="s">
+      <c r="B58" t="s" s="31">
         <v>47</v>
       </c>
     </row>
     <row r="59" spans="1:3">
-      <c r="B59" t="s">
+      <c r="B59" t="s" s="32">
         <v>48</v>
       </c>
     </row>
     <row r="60" spans="1:3">
-      <c r="B60" t="s">
+      <c r="B60" t="s" s="33">
         <v>49</v>
       </c>
     </row>

</xml_diff>